<commit_message>
--documentation --dataviz writing intro and built model parameterization graphic
</commit_message>
<xml_diff>
--- a/Documentation/Parameterized Model Table.xlsx
+++ b/Documentation/Parameterized Model Table.xlsx
@@ -126,12 +126,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -146,9 +152,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -166,6 +173,1762 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>300990</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E79B34D-319A-4905-BA3A-02353CA185D4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8412480" y="2213610"/>
+          <a:ext cx="1695450" cy="441960"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Spatial Networks [1]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>λ = 0 ------- 10</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>211455</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>312421</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{759E73C8-EA0E-4AB1-BD50-D8DD75FB821A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="5" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7682865" y="2647950"/>
+          <a:ext cx="741046" cy="468630"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FCDE18A-C28D-4BC3-B092-350BD99D6FD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6835140" y="3116580"/>
+          <a:ext cx="1695450" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Random Geometric    (Unit Disk) Graphs [2,3]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>R = 0 ------- 1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>537212</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19581644-5C7B-4C77-9D21-940471BA6AA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9284970" y="2655570"/>
+          <a:ext cx="3812" cy="449580"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5944AC5-9322-4B03-AC66-B74B5C3E9384}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8583930" y="3112770"/>
+          <a:ext cx="1695450" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Waxman Graphs [4,5]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" indent="0" algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>α = 0 ------- 10</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>72390</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>516255</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Straight Connector 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1AA6FAE-8705-4F2E-BBDC-1276AF4B5F0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="16" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10104120" y="2644140"/>
+          <a:ext cx="1083945" cy="472440"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>308610</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{14273CDE-8724-4E47-AD81-BFDDFB02FF5F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10340340" y="3116580"/>
+          <a:ext cx="1695450" cy="609600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Threshold Graphs [6]</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Θ = 0 ------- 10</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>211455</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>116205</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Straight Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F15B535B-6691-49F9-B773-D2F75329E490}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="5" idx="2"/>
+          <a:endCxn id="21" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7682865" y="3726180"/>
+          <a:ext cx="544830" cy="327660"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Rectangle 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8494873-5135-41DA-9F5A-7FF76838A2A3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7379970" y="4053840"/>
+          <a:ext cx="1695450" cy="617220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Soft Random</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Geometric  Graphs [7]</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>116205</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>40005</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Straight Connector 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA1900B-2389-420D-A1CF-16A950853BA9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="2"/>
+          <a:endCxn id="21" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8227695" y="3722370"/>
+          <a:ext cx="1203960" cy="331470"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>445770</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>220980</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Rectangle 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C1EDE5A-9B09-4150-81E2-9CE25D28A19B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9837420" y="4053840"/>
+          <a:ext cx="1695450" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Geometric Threshold</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Graphs [8,9]</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>13335</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>150495</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="32" name="Straight Connector 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B486D5EB-CCC5-413E-80D1-959B6336BEBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="31" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10685145" y="3726180"/>
+          <a:ext cx="777240" cy="327660"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>40005</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>13335</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="33" name="Straight Connector 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B0BBDC7-1FC4-4259-9AE5-2C3A12D47A9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="2"/>
+          <a:endCxn id="31" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9431655" y="3722370"/>
+          <a:ext cx="1253490" cy="331470"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>632460</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Straight Connector 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A86A2A2C-1C31-4E64-BF75-90F9BACF4840}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11304270" y="4514850"/>
+          <a:ext cx="7622" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>232410</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="46" name="Rectangle 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A695F81-A56B-4C74-B9B5-3C9A859AAD94}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11022330" y="4804410"/>
+          <a:ext cx="521970" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>α = 1 </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>541020</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="47" name="Rectangle 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1051EC38-2B70-4D95-9D64-89F44DC1ABAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10808970" y="5257800"/>
+          <a:ext cx="1043940" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Boolean Model [11]</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>624840</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>125730</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>632462</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="48" name="Straight Connector 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E82DA3A0-D08C-4F5A-BD15-01B3D2777ECC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="11296650" y="5063490"/>
+          <a:ext cx="7622" cy="186690"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>163830</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>171452</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Straight Connector 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFCDDB80-EE36-4498-9AA8-09DDD907AAE1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10195560" y="4518660"/>
+          <a:ext cx="7622" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>521970</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="Rectangle 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8695F538-5CF4-4731-8E0A-E924A4595C6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9913620" y="4808220"/>
+          <a:ext cx="521970" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>α = 2 </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>308610</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>72390</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="Rectangle 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C7E901C-7CE5-46E4-A830-CAEEB027527F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9700260" y="5261610"/>
+          <a:ext cx="1043940" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Gravity   Model [10]</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>156210</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>163832</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F5D8545-34B9-430C-B11C-9697DEC59C4A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10187940" y="5067300"/>
+          <a:ext cx="7622" cy="186690"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>11432</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>41910</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="58" name="Straight Connector 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A3043C6-B8F9-4D28-A950-EC0280E1E964}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="9395460" y="3726180"/>
+          <a:ext cx="7622" cy="2167890"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>72390</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>80010</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>83822</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="60" name="Straight Connector 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{627FFE81-07C5-49CE-933C-C7B29893EE79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="12024360" y="3737610"/>
+          <a:ext cx="11432" cy="3025140"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3812</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Straight Connector 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{64CC88CA-EB26-403B-BF5A-B29C5C1578AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6831330" y="3718560"/>
+          <a:ext cx="3812" cy="3059430"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>217170</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>110490</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="Rectangle 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42190A45-C4E2-4009-8F2F-F0F311DB3967}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8553450" y="5871210"/>
+          <a:ext cx="1695450" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Thresholded Soft Random</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Geometric Graphs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1905</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="64" name="Straight Connector 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DC0E03A-9F6A-40D4-A8F9-C9F055EFAD52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="62" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6833235" y="6099810"/>
+          <a:ext cx="1720215" cy="3810"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>203836</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>68580</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="66" name="Straight Connector 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4175EBD8-DB74-493F-B2BC-08BC4BF84814}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10235566" y="6069330"/>
+          <a:ext cx="1784984" cy="11430"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Rectangle 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83E5BBBB-3FC1-4943-B7DD-F4135180FB61}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8591550" y="6545580"/>
+          <a:ext cx="1695450" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Thresholded Random</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Geometric Graphs</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>255270</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Straight Connector 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5424602F-26BF-4FB0-AA27-885E68B15111}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="70" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10287000" y="6770370"/>
+          <a:ext cx="1756410" cy="3810"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>636270</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>3810</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="77" name="Straight Connector 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5733797-E8C2-4C9D-8EDF-77A80A94992F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6827520" y="6766560"/>
+          <a:ext cx="1756410" cy="3810"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -467,417 +2230,419 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="32.47265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="8.83984375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>0</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>0</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>0</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>0.5</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="1">
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>0.5</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="1">
         <v>0</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0.5</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>0.5</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>1</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>0.5</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>2</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>0.5</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>0.5</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>0.5</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>1</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="1">
         <v>0</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" t="s">
+      <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>1</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="1">
         <v>0</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" t="s">
+      <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>1</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="1">
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>1</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="1">
         <v>1</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>1</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="1">
         <v>2</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
+      <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>2</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
+      <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>1</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
--documentation --research first draft of individual model writeups
</commit_message>
<xml_diff>
--- a/Documentation/Parameterized Model Table.xlsx
+++ b/Documentation/Parameterized Model Table.xlsx
@@ -117,13 +117,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -152,12 +158,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -246,7 +253,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>λ = 0 ------- 10</a:t>
+            <a:t>λ </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -359,7 +366,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Random Geometric    (Unit Disk) Graphs [2,3]</a:t>
+            <a:t>Random Geometric    Graphs [2,3]</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -374,7 +381,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>R = 0 ------- 1</a:t>
+            <a:t>R</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -500,7 +507,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>α = 0 ------- 10</a:t>
+            <a:t>P(d(u,v))</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -628,7 +635,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Θ = 0 ------- 10</a:t>
+            <a:t>Θ </a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -698,8 +705,8 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -715,7 +722,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7379970" y="4053840"/>
-          <a:ext cx="1695450" cy="617220"/>
+          <a:ext cx="1695450" cy="464820"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -980,480 +987,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>632460</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>2</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="40" name="Straight Connector 39">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A86A2A2C-1C31-4E64-BF75-90F9BACF4840}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="11304270" y="4514850"/>
-          <a:ext cx="7622" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>350520</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>232410</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="Rectangle 45">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A695F81-A56B-4C74-B9B5-3C9A859AAD94}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11022330" y="4804410"/>
-          <a:ext cx="521970" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>α = 1 </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>137160</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>541020</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="Rectangle 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1051EC38-2B70-4D95-9D64-89F44DC1ABAC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10808970" y="5257800"/>
-          <a:ext cx="1043940" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Boolean Model [11]</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>624840</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>125730</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>632462</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="48" name="Straight Connector 47">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E82DA3A0-D08C-4F5A-BD15-01B3D2777ECC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="11296650" y="5063490"/>
-          <a:ext cx="7622" cy="186690"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>163830</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>171452</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="50" name="Straight Connector 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFCDDB80-EE36-4498-9AA8-09DDD907AAE1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="10195560" y="4518660"/>
-          <a:ext cx="7622" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>521970</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="Rectangle 50">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8695F538-5CF4-4731-8E0A-E924A4595C6A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9913620" y="4808220"/>
-          <a:ext cx="521970" cy="266700"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>α = 2 </a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>308610</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>140970</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>72390</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>49530</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="Rectangle 51">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C7E901C-7CE5-46E4-A830-CAEEB027527F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9700260" y="5261610"/>
-          <a:ext cx="1043940" cy="457200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Gravity   Model [10]</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="0"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>156210</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>163832</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="53" name="Straight Connector 52">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F5D8545-34B9-430C-B11C-9697DEC59C4A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="10187940" y="5067300"/>
-          <a:ext cx="7622" cy="186690"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>3810</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>68580</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>11432</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>41910</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1468,8 +1011,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="9395460" y="3726180"/>
-          <a:ext cx="7622" cy="2167890"/>
+          <a:off x="9391650" y="3726180"/>
+          <a:ext cx="11432" cy="1219200"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1495,15 +1038,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>72390</xdr:colOff>
+      <xdr:colOff>60960</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>80010</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>83822</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1518,8 +1061,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="12024360" y="3737610"/>
-          <a:ext cx="11432" cy="3025140"/>
+          <a:off x="12012930" y="3737610"/>
+          <a:ext cx="22862" cy="2072640"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1545,15 +1088,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>3812</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>3812</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>11430</xdr:rowOff>
+      <xdr:colOff>26670</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>140970</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1567,9 +1110,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="6831330" y="3718560"/>
-          <a:ext cx="3812" cy="3059430"/>
+        <a:xfrm>
+          <a:off x="6835142" y="3718560"/>
+          <a:ext cx="22858" cy="2091690"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1595,15 +1138,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>217170</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>110490</xdr:rowOff>
+      <xdr:colOff>194310</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1618,7 +1161,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8553450" y="5871210"/>
+          <a:off x="8530590" y="4953000"/>
           <a:ext cx="1695450" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1661,15 +1204,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1905</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>64770</xdr:rowOff>
+      <xdr:colOff>11430</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1685,9 +1228,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="6833235" y="6099810"/>
-          <a:ext cx="1720215" cy="3810"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6842760" y="5173980"/>
+          <a:ext cx="1687830" cy="7620"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1714,14 +1257,14 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>203836</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>34290</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>72390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>68580</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1736,7 +1279,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10235566" y="6069330"/>
+          <a:off x="10235566" y="5193030"/>
           <a:ext cx="1784984" cy="11430"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -1763,15 +1306,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:colOff>422910</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>255270</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1786,7 +1329,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8591550" y="6545580"/>
+          <a:off x="8534400" y="5574030"/>
           <a:ext cx="1695450" cy="457200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1829,15 +1372,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>255270</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1854,8 +1397,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="10287000" y="6770370"/>
-          <a:ext cx="1756410" cy="3810"/>
+          <a:off x="10229850" y="5791200"/>
+          <a:ext cx="1798320" cy="11430"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1880,16 +1423,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>636270</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>472440</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>156210</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1903,9 +1446,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="6827520" y="6766560"/>
-          <a:ext cx="1756410" cy="3810"/>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6835140" y="5806440"/>
+          <a:ext cx="1687830" cy="19050"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1928,6 +1471,135 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>575310</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="137538" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="19" name="TextBox 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0CACBB7-DE70-4E85-A7D0-70E8868AC89F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6766560" y="3705225"/>
+              <a:ext cx="137538" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>≤</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="19" name="TextBox 18">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0CACBB7-DE70-4E85-A7D0-70E8868AC89F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6766560" y="3705225"/>
+              <a:ext cx="137538" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>≤</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2228,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2515,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>25</v>
       </c>
@@ -2529,7 +2201,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>26</v>
       </c>
@@ -2543,7 +2215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -2557,7 +2229,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
@@ -2571,7 +2243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -2585,7 +2257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -2599,7 +2271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
@@ -2613,7 +2285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>14</v>
       </c>
@@ -2627,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -2641,8 +2313,12 @@
         <v>1</v>
       </c>
     </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="G26" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
--simulation --refactor --documentation trialing dynamic model simulations
</commit_message>
<xml_diff>
--- a/Documentation/Parameterized Model Table.xlsx
+++ b/Documentation/Parameterized Model Table.xlsx
@@ -498,7 +498,7 @@
         <a:p>
           <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1">
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -507,8 +507,41 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>P(d(u,v))</a:t>
+            <a:t>P(d</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="-25000">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>ij</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1471,135 +1504,6 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>575310</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="137538" cy="172227"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="19" name="TextBox 18">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0CACBB7-DE70-4E85-A7D0-70E8868AC89F}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6766560" y="3705225"/>
-              <a:ext cx="137538" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>≤</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="19" name="TextBox 18">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0CACBB7-DE70-4E85-A7D0-70E8868AC89F}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6766560" y="3705225"/>
-              <a:ext cx="137538" cy="172227"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>≤</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1902,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
--simulating building robustness metric
</commit_message>
<xml_diff>
--- a/Documentation/Parameterized Model Table.xlsx
+++ b/Documentation/Parameterized Model Table.xlsx
@@ -498,7 +498,7 @@
         <a:p>
           <a:pPr marL="0" indent="0" algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+            <a:rPr lang="en-US" sz="1100" b="1" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -510,7 +510,7 @@
             <a:t>P(d</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0" baseline="-25000">
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" baseline="-25000">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -522,7 +522,7 @@
             <a:t>ij</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="0" i="0">
+            <a:rPr lang="en-US" sz="1100" b="1" i="0">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
               </a:solidFill>
@@ -1806,8 +1806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>